<commit_message>
updates to prompteval and main script
</commit_message>
<xml_diff>
--- a/src/data/reqs_df_with_revisions.xlsx
+++ b/src/data/reqs_df_with_revisions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/github_projects/venv_aiswre/aiswre/aiswre/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/github_projects/venv_aiswre/aiswre/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_29E961FCF613C8264F2C4C35E5BAE4EA4C7A6657" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_29E961FCF613C8264F2C4C35E5BAE4EA4C7A6657" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FB82159-9C73-40DF-BF8B-F9F9ACC46E1A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30780" yWindow="2535" windowWidth="18900" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Requirement_#</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Requirement</t>
-  </si>
-  <si>
-    <t>revision</t>
   </si>
   <si>
     <t>Revised_Requirement</t>
@@ -444,13 +441,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="236.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,11 +466,8 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -475,19 +475,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -495,19 +492,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -515,19 +509,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -535,19 +526,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -555,19 +543,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -575,19 +560,16 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -595,19 +577,16 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -615,16 +594,13 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>